<commit_message>
`excel`: update tests to account for XLS float handling
</commit_message>
<xml_diff>
--- a/resources/test/excel-xlsx.xlsx
+++ b/resources/test/excel-xlsx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeln\Documents\GitHub\qsv\resources\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelnatividad/Documents/GitHub/qsv/resources/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD17CB80-5B37-4663-8262-A01852D40E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADE60E9-54F9-AB4F-B5CF-C78C5F1DCBA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="13176" xr2:uid="{8A16ABEB-80F3-4626-911E-5EEBE2ECA548}"/>
+    <workbookView xWindow="10900" yWindow="4360" windowWidth="23260" windowHeight="13180" xr2:uid="{8A16ABEB-80F3-4626-911E-5EEBE2ECA548}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>URL</t>
   </si>
@@ -58,13 +58,59 @@
   </si>
   <si>
     <t>http://api.zippopotam.us/us/92802</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>not a date</t>
+  </si>
+  <si>
+    <t>http://api.zippopotam.us/us/10013</t>
+  </si>
+  <si>
+    <t>Manhattan</t>
+  </si>
+  <si>
+    <t>google.com</t>
+  </si>
+  <si>
+    <t>apple.com</t>
+  </si>
+  <si>
+    <t>amazon.com</t>
+  </si>
+  <si>
+    <t>Mountain View</t>
+  </si>
+  <si>
+    <t>Cupertino</t>
+  </si>
+  <si>
+    <t>Seattle</t>
+  </si>
+  <si>
+    <t>microsoft.com</t>
+  </si>
+  <si>
+    <t>Redmond</t>
+  </si>
+  <si>
+    <t>Wednesday, March 14, 2012</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="166" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +123,14 @@
       <color rgb="FFCE9178"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -96,16 +150,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -418,51 +484,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1AE47A-F25E-496F-9905-B3C064511375}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A2:A4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>42</v>
+      </c>
+      <c r="D2" s="2">
+        <v>37145.354166666664</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>3.14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
+      <c r="C4">
+        <v>3.14159265358979</v>
+      </c>
+      <c r="D4" s="2">
+        <v>44202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>1.5</v>
+      </c>
+      <c r="D5">
+        <v>123.45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>20.02</v>
+      </c>
+      <c r="D6" s="5">
+        <v>44381.918749999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>37</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>14.23</v>
+      </c>
+      <c r="D8" s="2">
+        <v>40982</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>14.201000000000001</v>
+      </c>
+      <c r="D9" s="7">
+        <v>40982.645833333336</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1" xr:uid="{3566E436-8AFD-A74C-92E1-08452D7D9820}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
`excel`: add --safe-column-names option
</commit_message>
<xml_diff>
--- a/resources/test/excel-xlsx.xlsx
+++ b/resources/test/excel-xlsx.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelnatividad/Documents/GitHub/qsv/resources/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADE60E9-54F9-AB4F-B5CF-C78C5F1DCBA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D716BA-04F6-FF4B-B4D8-9A9336710F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10900" yWindow="4360" windowWidth="23260" windowHeight="13180" xr2:uid="{8A16ABEB-80F3-4626-911E-5EEBE2ECA548}"/>
+    <workbookView xWindow="10900" yWindow="4360" windowWidth="25660" windowHeight="13180" activeTab="1" xr2:uid="{8A16ABEB-80F3-4626-911E-5EEBE2ECA548}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="safe_column_name_test" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t>URL</t>
   </si>
@@ -100,6 +101,64 @@
   </si>
   <si>
     <t>Wednesday, March 14, 2012</t>
+  </si>
+  <si>
+    <t>col1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  col with leading and trailing spaces.  </t>
+  </si>
+  <si>
+    <t>123_starts_with_123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With * / special ? ! Characters. </t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>!!!date???</t>
+  </si>
+  <si>
+    <t>ka</t>
+  </si>
+  <si>
+    <t>da</t>
+  </si>
+  <si>
+    <t>ba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   This is some text. With whitespaces.  </t>
+  </si>
+  <si>
+    <t>jumped over the lazy dog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     by the zigzag
+quarry site.   </t>
+  </si>
+  <si>
+    <t>lorem ipsum dolorem</t>
+  </si>
+  <si>
+    <t>Joel was here</t>
+  </si>
+  <si>
+    <t>The quick BROWN fox with a very long column name is now jumping over a lazy dog by the zigzag quarry site</t>
   </si>
 </sst>
 </file>
@@ -107,8 +166,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="166" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -154,7 +213,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -163,12 +222,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -486,7 +546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1AE47A-F25E-496F-9905-B3C064511375}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -568,7 +628,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
@@ -577,12 +637,12 @@
       <c r="C6">
         <v>20.02</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>44381.918749999997</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
@@ -591,12 +651,12 @@
       <c r="C7">
         <v>37</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
@@ -610,7 +670,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B9" t="s">
@@ -619,7 +679,7 @@
       <c r="C9">
         <v>14.201000000000001</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>40982.645833333336</v>
       </c>
     </row>
@@ -630,4 +690,182 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29274CAE-063E-3347-BAD2-C2F95F0FB58B}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" customWidth="1"/>
+    <col min="7" max="7" width="83.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>1.5</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="8">
+        <v>37145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="2">
+        <v>25023</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4">
+        <v>3.4</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5">
+        <v>3.14</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>1.2E-4</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6">
+        <v>654.34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
`excel`: add --safe-column-names option (#598)
* `excel`: add --safe-column-names option

* missing punctuation
</commit_message>
<xml_diff>
--- a/resources/test/excel-xlsx.xlsx
+++ b/resources/test/excel-xlsx.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelnatividad/Documents/GitHub/qsv/resources/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADE60E9-54F9-AB4F-B5CF-C78C5F1DCBA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D716BA-04F6-FF4B-B4D8-9A9336710F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10900" yWindow="4360" windowWidth="23260" windowHeight="13180" xr2:uid="{8A16ABEB-80F3-4626-911E-5EEBE2ECA548}"/>
+    <workbookView xWindow="10900" yWindow="4360" windowWidth="25660" windowHeight="13180" activeTab="1" xr2:uid="{8A16ABEB-80F3-4626-911E-5EEBE2ECA548}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="safe_column_name_test" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t>URL</t>
   </si>
@@ -100,6 +101,64 @@
   </si>
   <si>
     <t>Wednesday, March 14, 2012</t>
+  </si>
+  <si>
+    <t>col1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  col with leading and trailing spaces.  </t>
+  </si>
+  <si>
+    <t>123_starts_with_123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With * / special ? ! Characters. </t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>!!!date???</t>
+  </si>
+  <si>
+    <t>ka</t>
+  </si>
+  <si>
+    <t>da</t>
+  </si>
+  <si>
+    <t>ba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   This is some text. With whitespaces.  </t>
+  </si>
+  <si>
+    <t>jumped over the lazy dog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     by the zigzag
+quarry site.   </t>
+  </si>
+  <si>
+    <t>lorem ipsum dolorem</t>
+  </si>
+  <si>
+    <t>Joel was here</t>
+  </si>
+  <si>
+    <t>The quick BROWN fox with a very long column name is now jumping over a lazy dog by the zigzag quarry site</t>
   </si>
 </sst>
 </file>
@@ -107,8 +166,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="166" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -154,7 +213,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -163,12 +222,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -486,7 +546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1AE47A-F25E-496F-9905-B3C064511375}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -568,7 +628,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
@@ -577,12 +637,12 @@
       <c r="C6">
         <v>20.02</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>44381.918749999997</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
@@ -591,12 +651,12 @@
       <c r="C7">
         <v>37</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
@@ -610,7 +670,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B9" t="s">
@@ -619,7 +679,7 @@
       <c r="C9">
         <v>14.201000000000001</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>40982.645833333336</v>
       </c>
     </row>
@@ -630,4 +690,182 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29274CAE-063E-3347-BAD2-C2F95F0FB58B}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" customWidth="1"/>
+    <col min="7" max="7" width="83.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>1.5</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="8">
+        <v>37145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="2">
+        <v>25023</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4">
+        <v>3.4</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5">
+        <v>3.14</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>1.2E-4</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6">
+        <v>654.34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
`excel`: smarter date parsing for XLSX files; rename --safe-column-names to --safe-header-names
- with XLSX files, a cell will still be parsed as a date, even if its column is not in the --dates-whitelist if the cell format has been explicitly set to a date format
- rename --safe-column-names to --safe-header-names for consistency with other options that refer to column names as headers
</commit_message>
<xml_diff>
--- a/resources/test/excel-xlsx.xlsx
+++ b/resources/test/excel-xlsx.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelnatividad/Documents/GitHub/qsv/resources/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D716BA-04F6-FF4B-B4D8-9A9336710F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA515825-6332-834E-BB99-E483645F7BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10900" yWindow="4360" windowWidth="25660" windowHeight="13180" activeTab="1" xr2:uid="{8A16ABEB-80F3-4626-911E-5EEBE2ECA548}"/>
+    <workbookView xWindow="40200" yWindow="5100" windowWidth="19800" windowHeight="13180" activeTab="2" xr2:uid="{8A16ABEB-80F3-4626-911E-5EEBE2ECA548}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="safe_column_name_test" sheetId="2" r:id="rId2"/>
+    <sheet name="safe_header_name_test" sheetId="2" r:id="rId2"/>
+    <sheet name="date_test" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>URL</t>
   </si>
@@ -159,6 +160,21 @@
   </si>
   <si>
     <t>The quick BROWN fox with a very long column name is now jumping over a lazy dog by the zigzag quarry site</t>
+  </si>
+  <si>
+    <t>plaincol</t>
+  </si>
+  <si>
+    <t>Wednesday, Mar-14-2012</t>
+  </si>
+  <si>
+    <t>it will still parse the dates below as date even if plaincol is not in the default --dates-whitelist because the cell format was set to date</t>
+  </si>
+  <si>
+    <t>9/11/01 8:30 am</t>
+  </si>
+  <si>
+    <t>the date below is not parsed as a date coz we didn't explicitly set the cell format to a date format and "plaincol" is not in the --dates-whitelist</t>
   </si>
 </sst>
 </file>
@@ -213,7 +229,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -229,6 +245,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -696,7 +713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29274CAE-063E-3347-BAD2-C2F95F0FB58B}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -868,4 +885,71 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D5285B-83B5-FC48-8B54-0072F1930554}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="42.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="58" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
+        <v>29580</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>37145.354166666664</v>
+      </c>
+      <c r="B3" s="8">
+        <v>37145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4">
+        <v>37145.354166666664</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>37145</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
`excel`: smarter date parsing for XLSX files; rename --safe-column-names to --safe-header-names (#603)
- with XLSX files, a cell will still be parsed as a date, even if its column is not in the --dates-whitelist if the cell format has been explicitly set to a date format
- rename --safe-column-names to --safe-header-names for consistency with other options that refer to column names as headers
</commit_message>
<xml_diff>
--- a/resources/test/excel-xlsx.xlsx
+++ b/resources/test/excel-xlsx.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelnatividad/Documents/GitHub/qsv/resources/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D716BA-04F6-FF4B-B4D8-9A9336710F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA515825-6332-834E-BB99-E483645F7BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10900" yWindow="4360" windowWidth="25660" windowHeight="13180" activeTab="1" xr2:uid="{8A16ABEB-80F3-4626-911E-5EEBE2ECA548}"/>
+    <workbookView xWindow="40200" yWindow="5100" windowWidth="19800" windowHeight="13180" activeTab="2" xr2:uid="{8A16ABEB-80F3-4626-911E-5EEBE2ECA548}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="safe_column_name_test" sheetId="2" r:id="rId2"/>
+    <sheet name="safe_header_name_test" sheetId="2" r:id="rId2"/>
+    <sheet name="date_test" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>URL</t>
   </si>
@@ -159,6 +160,21 @@
   </si>
   <si>
     <t>The quick BROWN fox with a very long column name is now jumping over a lazy dog by the zigzag quarry site</t>
+  </si>
+  <si>
+    <t>plaincol</t>
+  </si>
+  <si>
+    <t>Wednesday, Mar-14-2012</t>
+  </si>
+  <si>
+    <t>it will still parse the dates below as date even if plaincol is not in the default --dates-whitelist because the cell format was set to date</t>
+  </si>
+  <si>
+    <t>9/11/01 8:30 am</t>
+  </si>
+  <si>
+    <t>the date below is not parsed as a date coz we didn't explicitly set the cell format to a date format and "plaincol" is not in the --dates-whitelist</t>
   </si>
 </sst>
 </file>
@@ -213,7 +229,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -229,6 +245,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -696,7 +713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29274CAE-063E-3347-BAD2-C2F95F0FB58B}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -868,4 +885,71 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D5285B-83B5-FC48-8B54-0072F1930554}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="42.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="58" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
+        <v>29580</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>37145.354166666664</v>
+      </c>
+      <c r="B3" s="8">
+        <v>37145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4">
+        <v>37145.354166666664</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>37145</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
`excel`: minor performance tweaks
- remove unnecessary allocations in hot loop
- compare to f64::EPSILON instead of 0.0
- also added test for data types
</commit_message>
<xml_diff>
--- a/resources/test/excel-xlsx.xlsx
+++ b/resources/test/excel-xlsx.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelnatividad/Documents/GitHub/qsv/resources/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelnatividad/Local/GitHub/qsv/resources/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA515825-6332-834E-BB99-E483645F7BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0DE76D-EB2F-8A4E-B347-C4EABB574D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40200" yWindow="5100" windowWidth="19800" windowHeight="13180" activeTab="2" xr2:uid="{8A16ABEB-80F3-4626-911E-5EEBE2ECA548}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{8A16ABEB-80F3-4626-911E-5EEBE2ECA548}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="safe_header_name_test" sheetId="2" r:id="rId2"/>
     <sheet name="date_test" sheetId="3" r:id="rId3"/>
+    <sheet name="data types" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
   <si>
     <t>URL</t>
   </si>
@@ -175,6 +176,69 @@
   </si>
   <si>
     <t>the date below is not parsed as a date coz we didn't explicitly set the cell format to a date format and "plaincol" is not in the --dates-whitelist</t>
+  </si>
+  <si>
+    <t>The</t>
+  </si>
+  <si>
+    <t>quick</t>
+  </si>
+  <si>
+    <t>brown</t>
+  </si>
+  <si>
+    <t>fox</t>
+  </si>
+  <si>
+    <t>jumped</t>
+  </si>
+  <si>
+    <t>🍔</t>
+  </si>
+  <si>
+    <t>is</t>
+  </si>
+  <si>
+    <t>💩</t>
+  </si>
+  <si>
+    <t>🙀</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>emojis</t>
+  </si>
+  <si>
+    <t>foreign</t>
+  </si>
+  <si>
+    <t>敏捷的棕色狐狸在森林里奔跑</t>
+  </si>
+  <si>
+    <t>Franz jagt im komplett verwahrlosten Taxi quer durch Bayern</t>
+  </si>
+  <si>
+    <t>Le rusé goupil franchit d'un bond le chien somnolent.</t>
+  </si>
+  <si>
+    <t>El rápido zorro marrón</t>
+  </si>
+  <si>
+    <t>いろはにほへとちりぬるをわかよたれそつねならむうゐのおくやまけふこえてあさきゆめみしゑひもせす</t>
   </si>
 </sst>
 </file>
@@ -229,7 +293,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -246,6 +310,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -891,7 +956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D5285B-83B5-FC48-8B54-0072F1930554}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -952,4 +1017,179 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ABC9476-5A4B-2D49-B685-D8D9891A1EF5}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8">
+        <v>37145</v>
+      </c>
+      <c r="E2" s="10">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1.32434354545454</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="8">
+        <v>45206</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0.98984953703703704</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.42354645656453399</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8">
+        <v>15317</v>
+      </c>
+      <c r="E4" s="10">
+        <v>1.2815162037037038</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>-54545.656575678498</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>37145.354166666664</v>
+      </c>
+      <c r="E5" s="10">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>-5446563454.4354601</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4">
+        <v>16655.34375</v>
+      </c>
+      <c r="E6" s="10">
+        <v>4.6296296296296293E-4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
`excel`: better cell error handling
before, we were returning the debug value, which didn't have the '#' prefix to clearly indicate its a cell error - i.e. `#DIV/0!` instead of `Div0`

This improves Excel error handling while I research how to get the "original value" of a cell that's causing the error as discussed in #1682
</commit_message>
<xml_diff>
--- a/resources/test/excel-xlsx.xlsx
+++ b/resources/test/excel-xlsx.xlsx
@@ -1,23 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelnatividad/Local/GitHub/qsv/resources/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0DE76D-EB2F-8A4E-B347-C4EABB574D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8410C640-13ED-F443-B272-2CC8B5E1050C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{8A16ABEB-80F3-4626-911E-5EEBE2ECA548}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{8A16ABEB-80F3-4626-911E-5EEBE2ECA548}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="safe_header_name_test" sheetId="2" r:id="rId2"/>
     <sheet name="date_test" sheetId="3" r:id="rId3"/>
     <sheet name="data types" sheetId="4" r:id="rId4"/>
+    <sheet name="cellerrors" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="testname">cellerrors!$C$6</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,8 +40,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
   <si>
     <t>URL</t>
   </si>
@@ -239,6 +265,12 @@
   </si>
   <si>
     <t>いろはにほへとちりぬるをわかよたれそつねならむうゐのおくやまけふこえてあさきゆめみしゑひもせす</t>
+  </si>
+  <si>
+    <t>col 2</t>
+  </si>
+  <si>
+    <t>column-3</t>
   </si>
 </sst>
 </file>
@@ -330,9 +362,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -370,7 +402,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -476,7 +508,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -618,7 +650,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1023,7 +1055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ABC9476-5A4B-2D49-B685-D8D9891A1EF5}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -1192,4 +1224,94 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CD24E5-BA9C-DD46-A8BD-DAD39269A9FF}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>100/-2</f>
+        <v>-50</v>
+      </c>
+      <c r="C2">
+        <f>SUM(A2:A6)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="e">
+        <f>100/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C3" t="e" cm="1">
+        <f t="array" ref="C3">4*te</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f>100/2</f>
+        <v>50</v>
+      </c>
+      <c r="C4">
+        <f>5*testname</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f>100/3</f>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f>100/4</f>
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
`tests`: expand excel error sheet
</commit_message>
<xml_diff>
--- a/resources/test/excel-xlsx.xlsx
+++ b/resources/test/excel-xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelnatividad/Local/GitHub/qsv/resources/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8410C640-13ED-F443-B272-2CC8B5E1050C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D025777D-1EC9-5B4D-AE55-63C4EF4426DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{8A16ABEB-80F3-4626-911E-5EEBE2ECA548}"/>
   </bookViews>
@@ -281,7 +281,7 @@
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,6 +299,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF454545"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -325,7 +332,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -343,6 +350,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1228,10 +1236,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CD24E5-BA9C-DD46-A8BD-DAD39269A9FF}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1310,6 +1318,20 @@
         <v>4</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="e">
+        <f>B7+12</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B7" s="9" t="e">
+        <f>C7+20</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C7" s="11" t="e" cm="1">
+        <f t="array" ref="C7">_xlfn._xlws.SORT(_xlfn.CHOOSECOLS(A3:B20, 3))</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
`tests`: add more excel error test cases
</commit_message>
<xml_diff>
--- a/resources/test/excel-xlsx.xlsx
+++ b/resources/test/excel-xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelnatividad/Local/GitHub/qsv/resources/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D025777D-1EC9-5B4D-AE55-63C4EF4426DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99896454-16A8-ED48-9284-BDC11F069517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{8A16ABEB-80F3-4626-911E-5EEBE2ECA548}"/>
   </bookViews>
@@ -34,6 +34,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -63,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="72">
   <si>
     <t>URL</t>
   </si>
@@ -271,6 +273,15 @@
   </si>
   <si>
     <t>column-3</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>wxyz</t>
   </si>
 </sst>
 </file>
@@ -1236,10 +1247,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CD24E5-BA9C-DD46-A8BD-DAD39269A9FF}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1332,6 +1343,42 @@
         <v>#VALUE!</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f>10+10</f>
+        <v>20</v>
+      </c>
+      <c r="C8" t="e">
+        <f>SUM(C2:C7)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" t="str">
+        <f>LOWER(B9)</f>
+        <v>hello</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
`tests`: update xlsx test file
</commit_message>
<xml_diff>
--- a/resources/test/excel-xlsx.xlsx
+++ b/resources/test/excel-xlsx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelnatividad/Local/GitHub/qsv/resources/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelnatividad/GitHub/qsv/resources/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99896454-16A8-ED48-9284-BDC11F069517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33950FD-9EC6-8F4B-B31F-3ABDCC6F1A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{8A16ABEB-80F3-4626-911E-5EEBE2ECA548}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{8A16ABEB-80F3-4626-911E-5EEBE2ECA548}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,11 @@
     <sheet name="date_test" sheetId="3" r:id="rId3"/>
     <sheet name="data types" sheetId="4" r:id="rId4"/>
     <sheet name="cellerrors" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="testname">cellerrors!$C$6</definedName>
+    <definedName name="TestNamedRange">Sheet2!$C$20:$E$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="88">
   <si>
     <t>URL</t>
   </si>
@@ -282,6 +284,54 @@
   </si>
   <si>
     <t>wxyz</t>
+  </si>
+  <si>
+    <t>col2</t>
+  </si>
+  <si>
+    <t>col3</t>
+  </si>
+  <si>
+    <t>tabc1</t>
+  </si>
+  <si>
+    <t>tabc2</t>
+  </si>
+  <si>
+    <t>tabc3</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>a3</t>
+  </si>
+  <si>
+    <t>a4</t>
+  </si>
+  <si>
+    <t>a5</t>
+  </si>
+  <si>
+    <t>a6</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>charlie</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>echo</t>
   </si>
 </sst>
 </file>
@@ -378,6 +428,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{94B52031-BE65-9C4F-B97A-708620B54BCB}" name="Table1" displayName="Table1" ref="G11:I17" totalsRowShown="0">
+  <autoFilter ref="G11:I17" xr:uid="{94B52031-BE65-9C4F-B97A-708620B54BCB}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{E88EB8FE-7C56-9D4E-92C9-8B6FE59F07F1}" name="tabc1"/>
+    <tableColumn id="2" xr3:uid="{A3F64B36-2BE0-E143-A8AC-95F545C01FE8}" name="tabc2"/>
+    <tableColumn id="3" xr3:uid="{D6AC15FB-FA89-A94E-B09D-06C2C89ECA2F}" name="tabc3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1249,7 +1311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CD24E5-BA9C-DD46-A8BD-DAD39269A9FF}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1383,4 +1445,220 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9BC221-983A-EB4B-BC4B-EC0BE35C0C47}">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5">
+        <v>3.1456119999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>81</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>82</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0.99990000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22">
+        <v>3.3</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24">
+        <v>5.5</v>
+      </c>
+      <c r="E24">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
`excel`: add `--header-row` option
</commit_message>
<xml_diff>
--- a/resources/test/excel-xlsx.xlsx
+++ b/resources/test/excel-xlsx.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelnatividad/GitHub/qsv/resources/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelnatividad/Local/GitHub/qsv/resources/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33950FD-9EC6-8F4B-B31F-3ABDCC6F1A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F2B729-A898-4343-BC41-2E33B4272B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{8A16ABEB-80F3-4626-911E-5EEBE2ECA548}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="6" xr2:uid="{8A16ABEB-80F3-4626-911E-5EEBE2ECA548}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="data types" sheetId="4" r:id="rId4"/>
     <sheet name="cellerrors" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
+    <sheet name="firstnonemptyrow" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="testname">cellerrors!$C$6</definedName>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="89">
   <si>
     <t>URL</t>
   </si>
@@ -332,6 +333,9 @@
   </si>
   <si>
     <t>echo</t>
+  </si>
+  <si>
+    <t>col4</t>
   </si>
 </sst>
 </file>
@@ -1451,7 +1455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9BC221-983A-EB4B-BC4B-EC0BE35C0C47}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -1661,4 +1665,104 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{066830B7-C67B-4A48-AA5D-860676C22DB4}">
+  <dimension ref="A13:D18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16">
+        <v>3.3333330000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18">
+        <v>55.55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>